<commit_message>
epoch 1 transect update
</commit_message>
<xml_diff>
--- a/Oyster/transect/data/lc_trans_progress_people.xlsx
+++ b/Oyster/transect/data/lc_trans_progress_people.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="9855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="9855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="134">
   <si>
     <t>BTI1</t>
   </si>
@@ -331,6 +331,105 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>CKI1</t>
+  </si>
+  <si>
+    <t>CKI2</t>
+  </si>
+  <si>
+    <t>CKI3</t>
+  </si>
+  <si>
+    <t>CKN1</t>
+  </si>
+  <si>
+    <t>CKN2</t>
+  </si>
+  <si>
+    <t>CKN3</t>
+  </si>
+  <si>
+    <t>CKO1</t>
+  </si>
+  <si>
+    <t>CKO2</t>
+  </si>
+  <si>
+    <t>CKO3</t>
+  </si>
+  <si>
+    <t>CRI1</t>
+  </si>
+  <si>
+    <t>CRI2</t>
+  </si>
+  <si>
+    <t>CRI3</t>
+  </si>
+  <si>
+    <t>CRN1</t>
+  </si>
+  <si>
+    <t>CRN2</t>
+  </si>
+  <si>
+    <t>CRN3</t>
+  </si>
+  <si>
+    <t>CRO1</t>
+  </si>
+  <si>
+    <t>CRO2</t>
+  </si>
+  <si>
+    <t>CRO3</t>
+  </si>
+  <si>
+    <t>CRO4</t>
+  </si>
+  <si>
+    <t>HBI1</t>
+  </si>
+  <si>
+    <t>HBI2</t>
+  </si>
+  <si>
+    <t>HBI3</t>
+  </si>
+  <si>
+    <t>HBI4</t>
+  </si>
+  <si>
+    <t>HBN1</t>
+  </si>
+  <si>
+    <t>HBN2</t>
+  </si>
+  <si>
+    <t>HBN3</t>
+  </si>
+  <si>
+    <t>HBN5</t>
+  </si>
+  <si>
+    <t>HBN6</t>
+  </si>
+  <si>
+    <t>HBO1</t>
+  </si>
+  <si>
+    <t>HBO2</t>
+  </si>
+  <si>
+    <t>HBO3</t>
+  </si>
+  <si>
+    <t>Tyler Ring</t>
+  </si>
+  <si>
+    <t>Emily Colson</t>
   </si>
 </sst>
 </file>
@@ -661,11 +760,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S116"/>
+  <dimension ref="A1:S148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S95" sqref="S95"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3030,6 +3129,475 @@
         <v>43457</v>
       </c>
     </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B117" s="1">
+        <v>1</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E117" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F117" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B118" s="1">
+        <v>1</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E118" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F118" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B119" s="1">
+        <v>1</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E119" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F119" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B120" s="1">
+        <v>1</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E120" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B121" s="1">
+        <v>1</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E122" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B123" s="1">
+        <v>1</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E123" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B124" s="1">
+        <v>1</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E124" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" s="1">
+        <v>1</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E125" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B126" s="1">
+        <v>1</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E126" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F126" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B127" s="1">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E127" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F127" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B128" s="1">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E128" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F128" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" s="1">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F129" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B130" s="1">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E130" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F130" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B131" s="1">
+        <v>1</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E131" s="3">
+        <v>43613</v>
+      </c>
+      <c r="F131" s="3">
+        <v>43616</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B132" s="1">
+        <v>1</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E132" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B133" s="1">
+        <v>1</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E133" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B134" s="1">
+        <v>1</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E134" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B135" s="1">
+        <v>1</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E135" s="3">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B136" s="1">
+        <v>1</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E136" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B137" s="1">
+        <v>1</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B138" s="1">
+        <v>1</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E138" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B139" s="1">
+        <v>1</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E139" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B140" s="1">
+        <v>1</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B141" s="1">
+        <v>1</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E141" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B142" s="1">
+        <v>1</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E142" s="3"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B143" s="1">
+        <v>1</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E143" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B144" s="1">
+        <v>1</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E144" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B145" s="1">
+        <v>1</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E145" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B146" s="1">
+        <v>1</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E146" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B147" s="1">
+        <v>1</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E147" s="3">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B148" s="1">
+        <v>1</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E148" s="3"/>
+    </row>
   </sheetData>
   <sortState ref="A2:J118">
     <sortCondition ref="A2:A118"/>
@@ -3041,10 +3609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3988,6 +4556,46 @@
         <v>78</v>
       </c>
     </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B118" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B119" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B120" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B121" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B122" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B48"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update with last sampling event
</commit_message>
<xml_diff>
--- a/Oyster/transect/data/lc_trans_progress_people.xlsx
+++ b/Oyster/transect/data/lc_trans_progress_people.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="9855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="136">
   <si>
     <t>BTI1</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>Emily Colson</t>
+  </si>
+  <si>
+    <t>Tyler Coleman</t>
+  </si>
+  <si>
+    <t>Eric Bovee</t>
   </si>
 </sst>
 </file>
@@ -762,9 +768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I121" sqref="I121"/>
+      <selection pane="bottomLeft" activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3193,6 +3199,9 @@
       <c r="E120" s="3">
         <v>43613</v>
       </c>
+      <c r="F120" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
@@ -3207,6 +3216,9 @@
       <c r="E121" s="3">
         <v>43613</v>
       </c>
+      <c r="F121" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
@@ -3221,6 +3233,9 @@
       <c r="E122" s="3">
         <v>43613</v>
       </c>
+      <c r="F122" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
@@ -3235,6 +3250,9 @@
       <c r="E123" s="3">
         <v>43613</v>
       </c>
+      <c r="F123" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
@@ -3249,6 +3267,9 @@
       <c r="E124" s="3">
         <v>43613</v>
       </c>
+      <c r="F124" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
@@ -3263,6 +3284,9 @@
       <c r="E125" s="3">
         <v>43613</v>
       </c>
+      <c r="F125" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
@@ -3379,6 +3403,9 @@
       <c r="E132" s="3">
         <v>43613</v>
       </c>
+      <c r="F132" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -3393,6 +3420,9 @@
       <c r="E133" s="3">
         <v>43613</v>
       </c>
+      <c r="F133" s="3">
+        <v>43630</v>
+      </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
@@ -3407,6 +3437,7 @@
       <c r="E134" s="3">
         <v>43613</v>
       </c>
+      <c r="F134" s="3"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
@@ -3420,6 +3451,9 @@
       </c>
       <c r="E135" s="3">
         <v>43613</v>
+      </c>
+      <c r="F135" s="3">
+        <v>43630</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -3609,10 +3643,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124:A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4596,6 +4630,54 @@
         <v>133</v>
       </c>
     </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>43630</v>
+      </c>
+      <c r="B123" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>43630</v>
+      </c>
+      <c r="B124" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>43630</v>
+      </c>
+      <c r="B125" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>43630</v>
+      </c>
+      <c r="B126" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>43630</v>
+      </c>
+      <c r="B127" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>43630</v>
+      </c>
+      <c r="B128" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B48"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update figs and prep data tables
</commit_message>
<xml_diff>
--- a/Oyster/transect/data/lc_trans_progress_people.xlsx
+++ b/Oyster/transect/data/lc_trans_progress_people.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="9855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -771,9 +771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P162" sqref="P162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I147" sqref="I147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3752,6 +3752,9 @@
       <c r="E148" s="3">
         <v>43429</v>
       </c>
+      <c r="F148" s="3">
+        <v>43648</v>
+      </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
@@ -3809,6 +3812,9 @@
       <c r="E151" s="3">
         <v>43429</v>
       </c>
+      <c r="F151" s="3">
+        <v>43648</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
@@ -3842,6 +3848,9 @@
       </c>
       <c r="E153" s="3">
         <v>43429</v>
+      </c>
+      <c r="F153" s="3">
+        <v>43648</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -3925,7 +3934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+    <sheetView topLeftCell="A116" workbookViewId="0">
       <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>

</xml_diff>